<commit_message>
date change code added
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Title</t>
   </si>
@@ -51,16 +51,28 @@
     <t>Add New Contact</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>testing</t>
-  </si>
-  <si>
     <t>PhD</t>
   </si>
   <si>
-    <t>ing</t>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>ash</t>
+  </si>
+  <si>
+    <t>rai</t>
+  </si>
+  <si>
+    <t>bac</t>
+  </si>
+  <si>
+    <t>iii</t>
+  </si>
+  <si>
+    <t>28-04-2028</t>
   </si>
 </sst>
 </file>
@@ -96,8 +108,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,7 +383,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -378,15 +391,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.88671875" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -408,8 +421,14 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -417,19 +436,25 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>